<commit_message>
Add another aprox 50 words on 20 JAN 2012
</commit_message>
<xml_diff>
--- a/Today_words.xlsx
+++ b/Today_words.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="19020" windowHeight="10875"/>
@@ -11,27 +11,17 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">subsequently </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTRAVAGANT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEDIOUS </t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,6 +35,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -67,9 +63,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,34 +361,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:B3"/>
+  <dimension ref="B1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2">
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
+    <row r="1" spans="2:3">
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="27" spans="3:3">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="2"/>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="2"/>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="55" spans="3:3">
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="3:3">
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add aprox 50 words in Today_words sheet. Mostly words belong to C alphabate category
</commit_message>
<xml_diff>
--- a/Today_words.xlsx
+++ b/Today_words.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="19020" windowHeight="10875"/>
@@ -11,12 +11,346 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
+  <si>
+    <t>granularity</t>
+  </si>
+  <si>
+    <t>दानेदार होना</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oversight </t>
+  </si>
+  <si>
+    <t>निरीक्षण</t>
+  </si>
+  <si>
+    <t>सुविधा</t>
+  </si>
+  <si>
+    <t>conveniently</t>
+  </si>
+  <si>
+    <t>compliment</t>
+  </si>
+  <si>
+    <t>प्रशंसा</t>
+  </si>
+  <si>
+    <t>complement</t>
+  </si>
+  <si>
+    <t>इज़ाफ़ा करना</t>
+  </si>
+  <si>
+    <t>शामिल करना</t>
+  </si>
+  <si>
+    <t>comprise</t>
+  </si>
+  <si>
+    <t>लिखना</t>
+  </si>
+  <si>
+    <t>Compose</t>
+  </si>
+  <si>
+    <t>concede</t>
+  </si>
+  <si>
+    <t>स्वीकार करना</t>
+  </si>
+  <si>
+    <t>concise</t>
+  </si>
+  <si>
+    <t>संक्षिप्त</t>
+  </si>
+  <si>
+    <t>Confer</t>
+  </si>
+  <si>
+    <t>प्रदान करना</t>
+  </si>
+  <si>
+    <t>विशेषज्ञ</t>
+  </si>
+  <si>
+    <t>connoisseur</t>
+  </si>
+  <si>
+    <t>से मिलकर</t>
+  </si>
+  <si>
+    <t>Consist of</t>
+  </si>
+  <si>
+    <t>Consist in</t>
+  </si>
+  <si>
+    <t>में शामिल</t>
+  </si>
+  <si>
+    <t>संगत</t>
+  </si>
+  <si>
+    <t>consistent</t>
+  </si>
+  <si>
+    <t>contagious</t>
+  </si>
+  <si>
+    <t>संक्रामक(pass by body)</t>
+  </si>
+  <si>
+    <t>infectious</t>
+  </si>
+  <si>
+    <t>संक्रामक(pass by air,water)</t>
+  </si>
+  <si>
+    <t>समकालीन</t>
+  </si>
+  <si>
+    <t>contemporary</t>
+  </si>
+  <si>
+    <t>तिरस्कार</t>
+  </si>
+  <si>
+    <t>contempt</t>
+  </si>
+  <si>
+    <t>योग्य</t>
+  </si>
+  <si>
+    <t>Worthy</t>
+  </si>
+  <si>
+    <t>नित्य</t>
+  </si>
+  <si>
+    <t>Continual</t>
+  </si>
+  <si>
+    <t>convenience</t>
+  </si>
+  <si>
+    <t>रस्सी</t>
+  </si>
+  <si>
+    <t>chord</t>
+  </si>
+  <si>
+    <t>cord</t>
+  </si>
+  <si>
+    <t>तार</t>
+  </si>
+  <si>
+    <t>corporal punishment</t>
+  </si>
+  <si>
+    <t>शारीरिक दंड</t>
+  </si>
+  <si>
+    <t>बड़ा वकील</t>
+  </si>
+  <si>
+    <t>barrister</t>
+  </si>
+  <si>
+    <t>council</t>
+  </si>
+  <si>
+    <t>A COUNCIL is a board of elected representatives</t>
+  </si>
+  <si>
+    <t>counsel</t>
+  </si>
+  <si>
+    <t>Advice</t>
+  </si>
+  <si>
+    <t>जाली</t>
+  </si>
+  <si>
+    <t>counterfeit</t>
+  </si>
+  <si>
+    <t>विनम्र</t>
+  </si>
+  <si>
+    <t>courteous</t>
+  </si>
+  <si>
+    <t>विश्वसनीय</t>
+  </si>
+  <si>
+    <t>credible</t>
+  </si>
+  <si>
+    <t>संकट</t>
+  </si>
+  <si>
+    <t>crisis</t>
+  </si>
+  <si>
+    <t>कसौटी</t>
+  </si>
+  <si>
+    <t>criterion</t>
+  </si>
+  <si>
+    <t>आलोचना करना</t>
+  </si>
+  <si>
+    <t>criticise</t>
+  </si>
+  <si>
+    <t>महत्वपूर्ण</t>
+  </si>
+  <si>
+    <t>crucial</t>
+  </si>
+  <si>
+    <t>अलमारी</t>
+  </si>
+  <si>
+    <t>cupboard</t>
+  </si>
+  <si>
+    <t>जिज्ञासु</t>
+  </si>
+  <si>
+    <t>curious</t>
+  </si>
+  <si>
+    <t>जिज्ञासा</t>
+  </si>
+  <si>
+    <t>curiosity</t>
+  </si>
+  <si>
+    <t>किशमिश</t>
+  </si>
+  <si>
+    <t>currant</t>
+  </si>
+  <si>
+    <t>कार्यक्रम</t>
+  </si>
+  <si>
+    <t>curriculum</t>
+  </si>
+  <si>
+    <t>जीवन</t>
+  </si>
+  <si>
+    <t>vitae</t>
+  </si>
+  <si>
+    <t>बायोडेटा</t>
+  </si>
+  <si>
+    <t>curriculum vitae</t>
+  </si>
+  <si>
+    <t>curtain</t>
+  </si>
+  <si>
+    <t>पर्दा</t>
+  </si>
+  <si>
+    <t>पक्का</t>
+  </si>
+  <si>
+    <t>CERTAIN</t>
+  </si>
+  <si>
+    <t>निर्दयी</t>
+  </si>
+  <si>
+    <t>callous</t>
+  </si>
+  <si>
+    <t>तोप</t>
+  </si>
+  <si>
+    <t>cannon</t>
+  </si>
+  <si>
+    <t>cleric</t>
+  </si>
+  <si>
+    <t>पुरोहित</t>
+  </si>
+  <si>
+    <t>ढलाईकार</t>
+  </si>
+  <si>
+    <t>caster</t>
+  </si>
+  <si>
+    <t>नज़ला,सर्दी</t>
+  </si>
+  <si>
+    <t>ceiling</t>
+  </si>
+  <si>
+    <t>catarrh</t>
+  </si>
+  <si>
+    <t>उच्चतम सीमा,छत</t>
+  </si>
+  <si>
+    <t>अनाज - संबंधी</t>
+  </si>
+  <si>
+    <t>cereal</t>
+  </si>
+  <si>
+    <t>धारावाहिक</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>समारोह</t>
+  </si>
+  <si>
+    <t>ceremony</t>
+  </si>
+  <si>
+    <t>बचकाना</t>
+  </si>
+  <si>
+    <t>childish</t>
+  </si>
+  <si>
+    <t>बच्चों का सा</t>
+  </si>
+  <si>
+    <t>childlike</t>
+  </si>
+  <si>
+    <t>गँवार</t>
+  </si>
+  <si>
+    <t>coarse</t>
+  </si>
+  <si>
+    <t>बहुत भारी</t>
+  </si>
+  <si>
+    <t>colossal</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,92 +697,474 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C61"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3">
-      <c r="C1" s="2"/>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="2:3">
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="C16" s="2"/>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" s="2"/>
-    </row>
-    <row r="27" spans="3:3">
-      <c r="C27" s="2"/>
-    </row>
-    <row r="30" spans="3:3">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="3:3">
-      <c r="C31" s="2"/>
-    </row>
-    <row r="34" spans="3:3">
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="3:3">
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="3:3">
-      <c r="C36" s="2"/>
-    </row>
-    <row r="38" spans="3:3">
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="3:3">
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="3:3">
-      <c r="C40" s="2"/>
-    </row>
-    <row r="43" spans="3:3">
-      <c r="C43" s="2"/>
-    </row>
-    <row r="44" spans="3:3">
-      <c r="C44" s="2"/>
-    </row>
-    <row r="46" spans="3:3">
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="3:3">
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="3:3">
-      <c r="C48" s="2"/>
-    </row>
-    <row r="52" spans="3:3">
-      <c r="C52" s="2"/>
-    </row>
-    <row r="55" spans="3:3">
-      <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="3:3">
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="3:3">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="3:3">
+    <row r="58" spans="2:3">
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="3:3">
+    <row r="59" spans="2:3">
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="3:3">
+    <row r="60" spans="2:3">
       <c r="C60" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some words from office. All words are belong to E alphabate cat
</commit_message>
<xml_diff>
--- a/Today_words.xlsx
+++ b/Today_words.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="148">
   <si>
     <t>granularity</t>
   </si>
@@ -349,6 +349,117 @@
   </si>
   <si>
     <t>colossal</t>
+  </si>
+  <si>
+    <t>chasing</t>
+  </si>
+  <si>
+    <t>पीछा</t>
+  </si>
+  <si>
+    <t>earnest</t>
+  </si>
+  <si>
+    <t>ईमानदार</t>
+  </si>
+  <si>
+    <t>eerie</t>
+  </si>
+  <si>
+    <t>भयानक</t>
+  </si>
+  <si>
+    <t>टालना</t>
+  </si>
+  <si>
+    <t>elude</t>
+  </si>
+  <si>
+    <t>शर्मनाक</t>
+  </si>
+  <si>
+    <t>embarrassing</t>
+  </si>
+  <si>
+    <t>काट - छाँट करना</t>
+  </si>
+  <si>
+    <t>emend</t>
+  </si>
+  <si>
+    <t>ज़ोर देना</t>
+  </si>
+  <si>
+    <t>emphasise</t>
+  </si>
+  <si>
+    <t>endeavour</t>
+  </si>
+  <si>
+    <t>प्रयास</t>
+  </si>
+  <si>
+    <t>महापाप</t>
+  </si>
+  <si>
+    <t>enormity</t>
+  </si>
+  <si>
+    <t>enquiry(british)</t>
+  </si>
+  <si>
+    <t>Inquiry(American)</t>
+  </si>
+  <si>
+    <t>both are correct</t>
+  </si>
+  <si>
+    <t>ठीक कर लेना</t>
+  </si>
+  <si>
+    <t>insure(arrange for financial)</t>
+  </si>
+  <si>
+    <t>ensure</t>
+  </si>
+  <si>
+    <t>सुनिश्चित करना</t>
+  </si>
+  <si>
+    <t>अंत में</t>
+  </si>
+  <si>
+    <t>eventually</t>
+  </si>
+  <si>
+    <t>EXHAUSTED</t>
+  </si>
+  <si>
+    <t>थका</t>
+  </si>
+  <si>
+    <t>चिल्लाना</t>
+  </si>
+  <si>
+    <t>exclaim</t>
+  </si>
+  <si>
+    <t>explicit</t>
+  </si>
+  <si>
+    <t>स्पष्ट</t>
+  </si>
+  <si>
+    <t>अस्पष्ट</t>
+  </si>
+  <si>
+    <t>implicit</t>
+  </si>
+  <si>
+    <t>फिजूलखर्ची</t>
+  </si>
+  <si>
+    <t>extravagance</t>
   </si>
 </sst>
 </file>
@@ -397,10 +508,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,15 +808,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C60"/>
+  <dimension ref="B1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1156,16 +1269,154 @@
       </c>
     </row>
     <row r="57" spans="2:3">
-      <c r="C57" s="2"/>
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="58" spans="2:3">
-      <c r="C58" s="2"/>
+      <c r="B58" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="59" spans="2:3">
-      <c r="C59" s="2"/>
+      <c r="B59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="60" spans="2:3">
-      <c r="C60" s="2"/>
+      <c r="B60" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="B66" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3">
+      <c r="B67" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="2:3">
+      <c r="B68" t="s">
+        <v>133</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3">
+      <c r="B69" t="s">
+        <v>134</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3">
+      <c r="B70" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3">
+      <c r="B71" t="s">
+        <v>138</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3">
+      <c r="B72" t="s">
+        <v>141</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3">
+      <c r="B73" t="s">
+        <v>142</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3">
+      <c r="B75" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>146</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new 15 words from office belong to D cat
</commit_message>
<xml_diff>
--- a/Today_words.xlsx
+++ b/Today_words.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="19020" windowHeight="10875"/>
@@ -16,7 +16,98 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>goodness sake</t>
+  </si>
+  <si>
+    <t>भलाई के</t>
+  </si>
+  <si>
+    <t>deceased</t>
+  </si>
+  <si>
+    <t>मृतक</t>
+  </si>
+  <si>
+    <t>रोगी</t>
+  </si>
+  <si>
+    <t>diseased</t>
+  </si>
+  <si>
+    <t>छल</t>
+  </si>
+  <si>
+    <t>deceit</t>
+  </si>
+  <si>
+    <t>धोखा देना</t>
+  </si>
+  <si>
+    <t>deceive</t>
+  </si>
+  <si>
+    <t>सभ्य</t>
+  </si>
+  <si>
+    <t>decent</t>
+  </si>
+  <si>
+    <t>descent</t>
+  </si>
+  <si>
+    <t>अवरोह</t>
+  </si>
+  <si>
+    <t>संकेतमय</t>
+  </si>
+  <si>
+    <t>ALLUSION</t>
+  </si>
+  <si>
+    <t>DELUSION</t>
+  </si>
+  <si>
+    <t>भ्रम</t>
+  </si>
+  <si>
+    <t>सूखा</t>
+  </si>
+  <si>
+    <t>desiccated</t>
+  </si>
+  <si>
+    <t>निराश</t>
+  </si>
+  <si>
+    <t>desperate</t>
+  </si>
+  <si>
+    <t>अलग</t>
+  </si>
+  <si>
+    <t>detached</t>
+  </si>
+  <si>
+    <t>आपदा</t>
+  </si>
+  <si>
+    <t>disaster</t>
+  </si>
+  <si>
+    <t>disasterous</t>
+  </si>
+  <si>
+    <t>विनाशकारी</t>
+  </si>
+  <si>
+    <t>विचारशील</t>
+  </si>
+  <si>
+    <t>discreet</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,35 +454,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C75"/>
+  <dimension ref="B1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C68" sqref="B1:C75"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="2:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="2:3">
-      <c r="B2" s="1"/>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="7" spans="2:3">
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C7" s="2"/>
-    </row>
-    <row r="11" spans="2:3">
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C11" s="2"/>
-    </row>
-    <row r="16" spans="2:3">
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
       <c r="C16" s="2"/>
     </row>
     <row r="19" spans="3:3">
@@ -456,9 +656,6 @@
     </row>
     <row r="48" spans="3:3">
       <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="3:3">
-      <c r="C49" s="2"/>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" s="2"/>

</xml_diff>

<commit_message>
Add some words with memory key
</commit_message>
<xml_diff>
--- a/Today_words.xlsx
+++ b/Today_words.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="19020" windowHeight="10875"/>
@@ -16,98 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>goodness sake</t>
-  </si>
-  <si>
-    <t>भलाई के</t>
-  </si>
-  <si>
-    <t>deceased</t>
-  </si>
-  <si>
-    <t>मृतक</t>
-  </si>
-  <si>
-    <t>रोगी</t>
-  </si>
-  <si>
-    <t>diseased</t>
-  </si>
-  <si>
-    <t>छल</t>
-  </si>
-  <si>
-    <t>deceit</t>
-  </si>
-  <si>
-    <t>धोखा देना</t>
-  </si>
-  <si>
-    <t>deceive</t>
-  </si>
-  <si>
-    <t>सभ्य</t>
-  </si>
-  <si>
-    <t>decent</t>
-  </si>
-  <si>
-    <t>descent</t>
-  </si>
-  <si>
-    <t>अवरोह</t>
-  </si>
-  <si>
-    <t>संकेतमय</t>
-  </si>
-  <si>
-    <t>ALLUSION</t>
-  </si>
-  <si>
-    <t>DELUSION</t>
-  </si>
-  <si>
-    <t>भ्रम</t>
-  </si>
-  <si>
-    <t>सूखा</t>
-  </si>
-  <si>
-    <t>desiccated</t>
-  </si>
-  <si>
-    <t>निराश</t>
-  </si>
-  <si>
-    <t>desperate</t>
-  </si>
-  <si>
-    <t>अलग</t>
-  </si>
-  <si>
-    <t>detached</t>
-  </si>
-  <si>
-    <t>आपदा</t>
-  </si>
-  <si>
-    <t>disaster</t>
-  </si>
-  <si>
-    <t>disasterous</t>
-  </si>
-  <si>
-    <t>विनाशकारी</t>
-  </si>
-  <si>
-    <t>विचारशील</t>
-  </si>
-  <si>
-    <t>discreet</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,8 +365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -468,128 +377,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="2"/>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="2" spans="2:4">
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="2"/>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
+      <c r="B4" s="1"/>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="2"/>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>24</v>
-      </c>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="2:4">
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
Add some words from office
</commit_message>
<xml_diff>
--- a/Today_words.xlsx
+++ b/Today_words.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="19020" windowHeight="10875"/>
@@ -16,7 +16,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Immutable</t>
+  </si>
+  <si>
+    <t>अडिग</t>
+  </si>
+  <si>
+    <t>परिवर्तनशील</t>
+  </si>
+  <si>
+    <t>Mutable</t>
+  </si>
+  <si>
+    <t>यह दर्शाता है</t>
+  </si>
+  <si>
+    <t>demonstrates</t>
+  </si>
+  <si>
+    <t>स्पष्ट रूप से</t>
+  </si>
+  <si>
+    <t>explicitly</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,7 +391,7 @@
   <dimension ref="B1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="A1:XFD1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -377,18 +402,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="2"/>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="2:4">
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C2" s="2"/>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="1"/>

</xml_diff>